<commit_message>
final changes in and latest draft of report
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters_Thesis_Work\Calibration_Positioning_project\GitRepo\Wide-Band-Receiver-Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CFA6D9-DC34-4441-8B01-2E43B46AD47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA7D445-A8AF-424F-A2E4-73A034633CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Distance between each patch in Rx Patch Antenna (DbPA)</t>
   </si>
@@ -87,66 +87,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t xml:space="preserve">    "TimeStep:"    "1"    "doas"    "-34"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "2"    "doas"    "-32"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "3"    " Failed "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "4"    "doas"    "-26"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "5"    "doas"    "-23"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "6"    "doas"    "-21"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "7"    "doas"    "-18"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "8"    "doas"    "-15"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "9"    "doas"    "-11"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "10"    "doas"    "-8"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "11"    "doas"    "-6"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "12"    "doas"    "-1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "13"    "doas"    "1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "14"    " Failed "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "15"    "doas"    "7"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "16"    "doas"    "10"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "17"    "doas"    "12"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "18"    "doas"    "15"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "19"    "doas"    "30"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    "TimeStep:"    "20"    "doas"    "33"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">DfL
 </t>
@@ -556,9 +496,6 @@
   </si>
   <si>
     <t>SrNo</t>
-  </si>
-  <si>
-    <t>Output from MUSIC Algorithm</t>
   </si>
   <si>
     <t>EndToMid</t>
@@ -568,6 +505,9 @@
   </si>
   <si>
     <t>BaseToAnt</t>
+  </si>
+  <si>
+    <t>Final Output from MUSIC Algorithm</t>
   </si>
 </sst>
 </file>
@@ -918,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1013,6 +953,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1302,7 @@
     <col min="28" max="28" width="12" customWidth="1"/>
     <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.140625" customWidth="1"/>
-    <col min="31" max="31" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="32.5703125" style="33" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="53" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="13.42578125" style="1" customWidth="1"/>
     <col min="37" max="37" width="4.28515625" bestFit="1" customWidth="1"/>
@@ -1367,93 +1310,93 @@
   <sheetData>
     <row r="1" spans="1:37" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="AA1" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA1" s="18" t="s">
-        <v>47</v>
       </c>
       <c r="AB1" s="4"/>
       <c r="AC1" s="16" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="AD1" s="4"/>
       <c r="AE1" s="4" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
@@ -1577,8 +1520,8 @@
       <c r="AC2" s="14">
         <v>15</v>
       </c>
-      <c r="AE2" t="s">
-        <v>6</v>
+      <c r="AE2" s="33">
+        <v>-27.9</v>
       </c>
       <c r="AI2" t="s">
         <v>1</v>
@@ -1697,8 +1640,8 @@
       <c r="AC3" s="14">
         <v>44</v>
       </c>
-      <c r="AE3" t="s">
-        <v>7</v>
+      <c r="AE3" s="33">
+        <v>-25.3</v>
       </c>
       <c r="AI3" t="s">
         <v>2</v>
@@ -1820,8 +1763,8 @@
       <c r="AC4" s="14">
         <v>66</v>
       </c>
-      <c r="AE4" t="s">
-        <v>8</v>
+      <c r="AE4" s="33">
+        <v>-22.6</v>
       </c>
       <c r="AI4" t="s">
         <v>3</v>
@@ -1944,11 +1887,11 @@
       <c r="AC5" s="14">
         <v>92</v>
       </c>
-      <c r="AE5" t="s">
-        <v>9</v>
+      <c r="AE5" s="33">
+        <v>-19.8</v>
       </c>
       <c r="AI5" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="AJ5" s="1">
         <v>106</v>
@@ -2067,11 +2010,11 @@
       <c r="AC6" s="14">
         <v>131</v>
       </c>
-      <c r="AE6" t="s">
-        <v>10</v>
+      <c r="AE6" s="33">
+        <v>-16.899999999999999</v>
       </c>
       <c r="AI6" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="AJ6" s="1">
         <v>175.5</v>
@@ -2190,11 +2133,11 @@
       <c r="AC7" s="14">
         <v>191</v>
       </c>
-      <c r="AE7" t="s">
-        <v>11</v>
+      <c r="AE7" s="33">
+        <v>-13.9</v>
       </c>
       <c r="AI7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="AJ7" s="1">
         <v>12.1</v>
@@ -2313,8 +2256,8 @@
       <c r="AC8" s="14">
         <v>227</v>
       </c>
-      <c r="AE8" t="s">
-        <v>12</v>
+      <c r="AE8" s="33">
+        <v>-10.8</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -2427,8 +2370,8 @@
       <c r="AC9" s="14">
         <v>258</v>
       </c>
-      <c r="AE9" t="s">
-        <v>13</v>
+      <c r="AE9" s="33">
+        <v>-7.7</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -2541,8 +2484,8 @@
       <c r="AC10" s="14">
         <v>287</v>
       </c>
-      <c r="AE10" t="s">
-        <v>14</v>
+      <c r="AE10" s="33">
+        <v>-4.5</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -2655,8 +2598,8 @@
       <c r="AC11" s="14">
         <v>321</v>
       </c>
-      <c r="AE11" t="s">
-        <v>15</v>
+      <c r="AE11" s="33">
+        <v>-1.3</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -2769,8 +2712,8 @@
       <c r="AC12" s="14">
         <v>358</v>
       </c>
-      <c r="AE12" t="s">
-        <v>16</v>
+      <c r="AE12" s="33">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -2883,8 +2826,8 @@
       <c r="AC13" s="14">
         <v>389</v>
       </c>
-      <c r="AE13" t="s">
-        <v>17</v>
+      <c r="AE13" s="33">
+        <v>5.2</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -2997,8 +2940,8 @@
       <c r="AC14" s="14">
         <v>419</v>
       </c>
-      <c r="AE14" t="s">
-        <v>18</v>
+      <c r="AE14" s="33">
+        <v>8.4</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -3111,8 +3054,8 @@
       <c r="AC15" s="14">
         <v>446</v>
       </c>
-      <c r="AE15" t="s">
-        <v>19</v>
+      <c r="AE15" s="33">
+        <v>11.5</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -3225,8 +3168,8 @@
       <c r="AC16" s="14">
         <v>476</v>
       </c>
-      <c r="AE16" t="s">
-        <v>20</v>
+      <c r="AE16" s="33">
+        <v>14.6</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -3339,8 +3282,8 @@
       <c r="AC17" s="14">
         <v>499</v>
       </c>
-      <c r="AE17" t="s">
-        <v>21</v>
+      <c r="AE17" s="33">
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -3453,8 +3396,8 @@
       <c r="AC18" s="14">
         <v>533</v>
       </c>
-      <c r="AE18" t="s">
-        <v>22</v>
+      <c r="AE18" s="33">
+        <v>20.5</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -3567,8 +3510,8 @@
       <c r="AC19" s="14">
         <v>573</v>
       </c>
-      <c r="AE19" t="s">
-        <v>23</v>
+      <c r="AE19" s="33">
+        <v>23.2</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -3681,8 +3624,8 @@
       <c r="AC20" s="14">
         <v>601</v>
       </c>
-      <c r="AE20" t="s">
-        <v>24</v>
+      <c r="AE20" s="33">
+        <v>25.9</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3795,8 +3738,8 @@
       <c r="AC21" s="15">
         <v>630</v>
       </c>
-      <c r="AE21" t="s">
-        <v>25</v>
+      <c r="AE21" s="33">
+        <v>28.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>